<commit_message>
Adding URLs for Selenium
</commit_message>
<xml_diff>
--- a/Report/URLs not fetched Selenium.xlsx
+++ b/Report/URLs not fetched Selenium.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pramod.setlur/Google Drive/USC Subjects/Information Retrieval/assignments/assignment 1/Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pramod.setlur/Google Drive/USC Subjects/Information Retrieval/assignments/assignment 1/nutch-crawling/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -30,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="113">
   <si>
     <t>URLS</t>
   </si>
   <si>
-    <t>List of URLs that we weren't able to fetch</t>
-  </si>
-  <si>
     <t>REASON</t>
   </si>
   <si>
@@ -62,42 +59,21 @@
     <t>http://nightforceoptics.com/current-promotions</t>
   </si>
   <si>
-    <t>http://images.gunsinternational.com/dyn/Winchester Collector.jpg</t>
-  </si>
-  <si>
     <t>java.lang.IllegalArgumentException</t>
   </si>
   <si>
-    <t>https://www.tcarms.com/venture-promo</t>
-  </si>
-  <si>
-    <t>javax.net.ssl.SSLProtocolException</t>
-  </si>
-  <si>
-    <t>http://sportsoptics.zeiss.com/content/dam/SportsOptics/usa/pdf/ZEI_4529_8.5x3.37_RebateBirdingUS_HR.pdf</t>
-  </si>
-  <si>
     <t>java.net.UnknownHostException</t>
   </si>
   <si>
-    <t>http://www.slickguns.com/sites/default/files/Ares Armor AR10 LR308 Nickel Boron Bolt Carrier Group at Granite Ridge Outfitters_thumb.jpg</t>
-  </si>
-  <si>
     <t>http://www.fflunleashed.com/comments/feed/</t>
   </si>
   <si>
     <t>http://www.slickguns.com/sites/default/files/</t>
   </si>
   <si>
-    <t>http://www.atf.treas.gov/pdfcon.htm</t>
-  </si>
-  <si>
     <t>java.net.NoRouteToHostException</t>
   </si>
   <si>
-    <t>http://images.gunsinternational.com/dyn/Turnbull Serious Leverage.jpg</t>
-  </si>
-  <si>
     <t>https://www.wildlife.ca.gov/</t>
   </si>
   <si>
@@ -134,12 +110,6 @@
     <t>http://www.gunsnammostore.com/p-68925-sw-811034-mp15-22-moe-sa-22-long-rifle-16-251-magpul-moe-stk-blk.aspx</t>
   </si>
   <si>
-    <t>http://www.gandermountain.com/Apparel/The-North-Face-Store/Camping-Gear</t>
-  </si>
-  <si>
-    <t>http://www.slickguns.com/sites/default/files/Screen Shot 2015-10-11 at 9.18.31 PM.jpg</t>
-  </si>
-  <si>
     <t>https://www.gunup.com/shop/dpms-308-oracle-flr-oc</t>
   </si>
   <si>
@@ -161,12 +131,6 @@
     <t>java.net.SocketException</t>
   </si>
   <si>
-    <t>http://www.kygunco.com/Springfield-1911-A1-TRP-Service-Black-45-ACP-5"-Barrel-7-1-1967</t>
-  </si>
-  <si>
-    <t>http://www.slickguns.com/users/protholl</t>
-  </si>
-  <si>
     <t>http://www.slickguns.com/sites/default/files/Radical762x39Rifle (12 of 13).jpg</t>
   </si>
   <si>
@@ -239,21 +203,6 @@
     <t>https://player.vimeo.com/video/130271202</t>
   </si>
   <si>
-    <t>http://www.slickguns.com/sites/default/files/VO Ratchet Red Dot Sight Acom 4.jpg</t>
-  </si>
-  <si>
-    <t>http://www.kingsfirearmsandmore.com/product.howard-leight-impact-sport-electronic-hearing-protection-82</t>
-  </si>
-  <si>
-    <t>http://www.slickguns.com/sites/default/files/VO Ratchet Red Dot Sight Acom 6.jpg</t>
-  </si>
-  <si>
-    <t>http://www.slickguns.com/sites/default/files/7 Romanian AK Draco Pistol 25-1676.jpg</t>
-  </si>
-  <si>
-    <t>http://www.mrgundealer.com/product.walther-ppq-m2-navy-sd-semi-automatic-double-action-full-9mm-4-polymer-black-15rd-17rd-2-mags-fixed-sights</t>
-  </si>
-  <si>
     <t>ttp://www.mrgundealer.com/product.kel-tec-plr22-plr-22-22lr-10-271-polymer-grip-black-finish</t>
   </si>
   <si>
@@ -263,18 +212,6 @@
     <t>http://www.slickguns.com/sites/default/files/Armor Wrench Quick Sheet8_no_background.jpg</t>
   </si>
   <si>
-    <t>http://images.gunsinternational.com/banners/SafariOutfittersLtd 180 x150 .jpg</t>
-  </si>
-  <si>
-    <t>http://www.slickguns.com/sites/default/files/Ultralight 30mm Scope Mount APRA210500 - Granite Ridge Outfitters.jpg</t>
-  </si>
-  <si>
-    <t>http://www.slickguns.com/sites/default/files/6 Romanian AK Draco Pistol 25-1676_thumb.jpg</t>
-  </si>
-  <si>
-    <t>https://www.gunup.com/shop/ruger-lcp-3701</t>
-  </si>
-  <si>
     <t>http://www.gandermountain.com/ugly-stik/images/ugly-stik-gx2-03.jpg</t>
   </si>
   <si>
@@ -302,27 +239,6 @@
     <t>https:/product-category/defense-spray/oc-spray/</t>
   </si>
   <si>
-    <t>http://mbdn.de/</t>
-  </si>
-  <si>
-    <t>http://www.kygunco.com/Taurus-444-Ultra-Lite-Titanium-Stainless-44-Mag-Revolver-2.25"-6-Round-25175</t>
-  </si>
-  <si>
-    <t>http://nikolay.bg/trunk/xmlrpc.php</t>
-  </si>
-  <si>
-    <t>http://old.statcounter.com/project/</t>
-  </si>
-  <si>
-    <t>HTTP 500</t>
-  </si>
-  <si>
-    <t>http://charlotteobserver.cinesport.com/placead</t>
-  </si>
-  <si>
-    <t>http://scorpiotechnologies.com /</t>
-  </si>
-  <si>
     <t>https://www.site5.com/d/email-dialog/</t>
   </si>
   <si>
@@ -347,15 +263,6 @@
     <t>http://www.plussizedressesx.com/</t>
   </si>
   <si>
-    <t>http://assets.winchesterdownload.com/Winchester Download Site Resources/Symbols/s22lrfsp/Consumer Site/S22LRFSP_EndView_thumbnail.png</t>
-  </si>
-  <si>
-    <t>http://www.stltoday.com/print-edition/</t>
-  </si>
-  <si>
-    <t>HTTP 417</t>
-  </si>
-  <si>
     <t>http://www.charlotteobserver.com/entertainment/blogs_columnists</t>
   </si>
   <si>
@@ -377,15 +284,6 @@
     <t>https://www.site5.com/d/no-worry-full-management/</t>
   </si>
   <si>
-    <t>http://www.webyshops.com/Policies/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://www.webyshops.com/Product-Type/Ammo-pt/record </t>
-  </si>
-  <si>
-    <t>HTTP 404</t>
-  </si>
-  <si>
     <t>https://www.site5.com/d/vps-backups/</t>
   </si>
   <si>
@@ -393,6 +291,84 @@
   </si>
   <si>
     <t>http://www.leelaecospa.ca/assets/light/spa-business award4-b46557dc07a2d5068eab28c4eb0a7bda.png</t>
+  </si>
+  <si>
+    <t>Crawled Successfully</t>
+  </si>
+  <si>
+    <t>http://www.ksl.com/?sid=28229430&amp;nid=148</t>
+  </si>
+  <si>
+    <t>https://www.dallasguns.com/guns_for_sale/Rock_Island/8764</t>
+  </si>
+  <si>
+    <t>http://www.gunbroker.com/Auction/ViewItem.aspx?Item=515079854</t>
+  </si>
+  <si>
+    <t>http://www.ksl.com/?sid=23777279</t>
+  </si>
+  <si>
+    <t>http://www.gunbroker.com/Auction/ViewItem.aspx?Item=515115454 </t>
+  </si>
+  <si>
+    <t>http://www.gunbroker.com/Auction/ViewItem.aspx?Item=515074091</t>
+  </si>
+  <si>
+    <t>https://www.dallasguns.com/guns_for_sale/SIG/9016</t>
+  </si>
+  <si>
+    <t>https://www.dallasguns.com/guns_for_sale/Military/6095</t>
+  </si>
+  <si>
+    <t>https://www.ksl.com/?sid=36650287&amp;nid=148</t>
+  </si>
+  <si>
+    <t>http://www.gunbroker.com/Auction/ViewItem.aspx?Item=511642067</t>
+  </si>
+  <si>
+    <t>https://www.dallasguns.com/guns_for_sale/Glock/364</t>
+  </si>
+  <si>
+    <t>https://www.dallasguns.com/guns_for_sale/Kimber/7270</t>
+  </si>
+  <si>
+    <t>https://www.dallasguns.com/guns_for_sale/Smith_Wesson/2512</t>
+  </si>
+  <si>
+    <t>https://www.dallasguns.com/guns_for_sale/CZ/11639</t>
+  </si>
+  <si>
+    <t>http://www.gunbroker.com/Auction/ViewItem.aspx?Item=515079648</t>
+  </si>
+  <si>
+    <t>http://www.ksl.com/?nid=148&amp;sid=23519836</t>
+  </si>
+  <si>
+    <t>http://www.ksl.com/index.php?sid=23636218&amp;nid=148&amp;title=gun-show-sees-</t>
+  </si>
+  <si>
+    <t>http://www.ksl.com/?nid=157&amp;sid=34682289</t>
+  </si>
+  <si>
+    <t>https://www.ksl.com/?sid=24229642</t>
+  </si>
+  <si>
+    <t>http://www.gunbroker.com/Auction/ViewItem.aspx?Item=515080637</t>
+  </si>
+  <si>
+    <t>http://www.ksl.com/?nid=157&amp;sid=33709768</t>
+  </si>
+  <si>
+    <t>http://www.ksl.com/?nid=157&amp;sid=36937438&amp;s_cid=rss-157</t>
+  </si>
+  <si>
+    <t>http://www.gunbroker.com/Auction/ViewItem.aspx?Item=511639966</t>
+  </si>
+  <si>
+    <t>List of URLs that we weren't able to crawl.</t>
+  </si>
+  <si>
+    <t>The ones marked in green were successfully crawled by our Selenium Custom Handlers.</t>
   </si>
 </sst>
 </file>
@@ -440,7 +416,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -450,6 +426,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,7 +452,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -503,6 +485,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -850,8 +835,8 @@
   </sheetPr>
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -871,7 +856,7 @@
     </row>
     <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="D2" s="6"/>
     </row>
@@ -886,840 +871,873 @@
       <c r="D4" s="7"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5"/>
-      <c r="D5" s="6"/>
+      <c r="D5" s="10" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="22.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>3</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>4</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>6</v>
       </c>
       <c r="D8"/>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>7</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>8</v>
       </c>
       <c r="D9"/>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>11</v>
+      <c r="B11" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>13</v>
+      <c r="B12" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>15</v>
+      <c r="B13" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>11</v>
+      <c r="B14" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>20</v>
+      <c r="B17" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>11</v>
+      <c r="B18" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>8</v>
+      <c r="B29" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>11</v>
+      <c r="B30" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="5" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>11</v>
+      <c r="B36" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>4</v>
+      <c r="B37" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="5" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="5" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="5" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="5" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="5" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="5" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="5" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="5" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B56" s="5" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="5" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="5" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" s="5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="5" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B61" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>11</v>
+      <c r="B61" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B62" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>8</v>
+      <c r="B62" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B63" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>11</v>
+      <c r="B63" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B64" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>11</v>
+      <c r="B64" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B65" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>8</v>
+      <c r="B65" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B66" s="5" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B67" s="5" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B68" s="5" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B69" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>11</v>
+      <c r="B69" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B70" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>11</v>
+      <c r="B70" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B71" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>11</v>
+      <c r="B71" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B72" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>37</v>
+      <c r="B72" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B73" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B74" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B75" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B76" s="5" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B77" s="5" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B78" s="5" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B79" s="5" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B80" s="5" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B81" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>4</v>
+      <c r="B81" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B82" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>11</v>
+      <c r="B82" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="83" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B83" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>6</v>
+      <c r="B83" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B84" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C84" s="9" t="s">
-        <v>94</v>
+      <c r="B84" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B85" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C85" s="9" t="s">
-        <v>4</v>
+      <c r="B85" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="86" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B86" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>11</v>
+      <c r="B86" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="87" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B87" s="5" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B88" s="5" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B89" s="5" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B90" s="5" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B91" s="5" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="92" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B92" s="5" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="93" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B93" s="5" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B94" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C94" s="9" t="s">
-        <v>11</v>
+      <c r="B94" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B95" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>107</v>
+      <c r="B95" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="96" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B96" s="5" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>101</v>
+        <v>73</v>
       </c>
     </row>
     <row r="97" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B97" s="5" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B98" s="5" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B99" s="5" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B100" s="5" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B101" s="5" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B102" s="5" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="C102" s="9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B103" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>8</v>
+      <c r="B103" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B104" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C104" s="9" t="s">
-        <v>117</v>
+      <c r="B104" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="105" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B105" s="5" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B106" s="5" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="C106" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B107" s="12" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B13" r:id="rId3"/>
+    <hyperlink ref="B14" r:id="rId4"/>
+    <hyperlink ref="B17" r:id="rId5"/>
+    <hyperlink ref="B18" r:id="rId6"/>
+    <hyperlink ref="B29" r:id="rId7"/>
+    <hyperlink ref="B37" r:id="rId8"/>
+    <hyperlink ref="B61" r:id="rId9"/>
+    <hyperlink ref="B65" r:id="rId10"/>
+    <hyperlink ref="B69" r:id="rId11"/>
+    <hyperlink ref="B71" r:id="rId12"/>
+    <hyperlink ref="B81" r:id="rId13"/>
+    <hyperlink ref="B84" r:id="rId14"/>
+    <hyperlink ref="B94" r:id="rId15"/>
+    <hyperlink ref="B104" r:id="rId16"/>
+    <hyperlink ref="B103" r:id="rId17"/>
+    <hyperlink ref="B95" r:id="rId18"/>
+    <hyperlink ref="B86" r:id="rId19"/>
+    <hyperlink ref="B85" r:id="rId20"/>
+    <hyperlink ref="B83" r:id="rId21"/>
+    <hyperlink ref="B82" r:id="rId22"/>
+    <hyperlink ref="B72" r:id="rId23"/>
+    <hyperlink ref="B70" r:id="rId24"/>
+    <hyperlink ref="B64" r:id="rId25"/>
+    <hyperlink ref="B63" r:id="rId26"/>
+    <hyperlink ref="B62" r:id="rId27"/>
+    <hyperlink ref="B36" r:id="rId28"/>
+    <hyperlink ref="B30" r:id="rId29"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.2" right="0.2" top="0.36" bottom="0.2" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId30"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>